<commit_message>
Cleaned Code, and added exporting from Insert Widnow
Cleaned code from insert window
Cleaned a coiple lines from reportsframe
</commit_message>
<xml_diff>
--- a/Excel/Form(1).xlsx
+++ b/Excel/Form(1).xlsx
@@ -12,29 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
-  <si>
-    <t>AssociationName</t>
-  </si>
-  <si>
-    <t>Year</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Aisle</t>
-  </si>
-  <si>
-    <t>Row</t>
-  </si>
-  <si>
-    <t>Column</t>
-  </si>
-  <si>
-    <t>Depth</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -83,30 +61,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2"/>
+    <row r="1"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>